<commit_message>
Update Unit 2 files.
</commit_message>
<xml_diff>
--- a/data/Earth_Land_Water.xlsx
+++ b/data/Earth_Land_Water.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10118"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/middletonk/Github/RDABR/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A0033A1-23B9-BB4B-B9B8-1D0E63E18B49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80531E25-23AD-3C49-ABEF-D57B191725D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1040" yWindow="1460" windowWidth="28100" windowHeight="17440" xr2:uid="{52A5458D-C65A-CB4B-BEE2-EC74A84C567C}"/>
+    <workbookView xWindow="35520" yWindow="1600" windowWidth="28100" windowHeight="17440" xr2:uid="{52A5458D-C65A-CB4B-BEE2-EC74A84C567C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -419,10 +419,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B773272-D551-834F-8B41-8F1BD2C8924B}">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -437,47 +437,47 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B2">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="B3">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B4">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B5">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B6">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B7">
         <v>9</v>
@@ -485,18 +485,26 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8">
+        <v>12</v>
+      </c>
+      <c r="B8">
         <v>13</v>
-      </c>
-      <c r="B8">
-        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9">
+        <v>13</v>
+      </c>
+      <c r="B9">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10">
         <v>15</v>
       </c>
-      <c r="B9">
-        <v>9</v>
+      <c r="B10">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>